<commit_message>
add fra report. update one trip length
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-10.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-10.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="428">
   <si>
     <t>Train ID</t>
   </si>
@@ -1335,6 +1335,9 @@
   </si>
   <si>
     <t>Train didn't fully stop at Station, onboard flashed prompts. Train was probably cut out to avoid confusion.</t>
+  </si>
+  <si>
+    <t>Train was not soft cut out at end of run</t>
   </si>
 </sst>
 </file>
@@ -1824,91 +1827,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -2270,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK163"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q60" sqref="Q60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A139" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R154" sqref="R154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2714,7 +2633,7 @@
         <v>140</v>
       </c>
       <c r="I6" s="30">
-        <v>42500.307696759257</v>
+        <v>42500.222372685188</v>
       </c>
       <c r="J6" s="61">
         <v>5</v>
@@ -2729,19 +2648,21 @@
       </c>
       <c r="M6" s="12">
         <f t="shared" si="1"/>
-        <v>0.11630787036847323</v>
+        <v>3.0983796299551614E-2</v>
       </c>
       <c r="N6" s="13">
         <f t="shared" ref="N6:N40" si="3">$M6*24*60</f>
-        <v>167.48333333060145</v>
+        <v>44.616666671354324</v>
       </c>
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
+      <c r="R6" s="62" t="s">
+        <v>427</v>
+      </c>
       <c r="T6" s="75" t="str">
         <f t="shared" ref="T6:T37" si="4">"https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'"&amp;TEXT(E6-1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600',mode:absolute,to:'"&amp;TEXT(I6+1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed',"&amp;"'Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:"&amp;"(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc."&amp;B6&amp;"%22')),sort:!(Time,asc))"</f>
-        <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-05-10 04:33:02-0600',mode:absolute,to:'2016-05-10 07:24:05-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4008%22')),sort:!(Time,asc))</v>
+        <v>https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'2016-05-10 04:33:02-0600',mode:absolute,to:'2016-05-10 05:21:13-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed','Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc.4008%22')),sort:!(Time,asc))</v>
       </c>
       <c r="U6" s="75" t="str">
         <f t="shared" ref="U6:U37" si="5">IF(Y6&lt;23,"Y","N")</f>
@@ -8133,7 +8054,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="Y70" s="75">
-        <f t="shared" ref="Y70:Y101" si="27">ABS(X70-W70)</f>
+        <f t="shared" ref="Y70:Y90" si="27">ABS(X70-W70)</f>
         <v>23.279700000000002</v>
       </c>
       <c r="Z70" s="76" t="e">
@@ -12931,7 +12852,7 @@
         <v>23.330400000000001</v>
       </c>
       <c r="Y127" s="75">
-        <f t="shared" ref="Y127:Y158" si="52">ABS(X127-W127)</f>
+        <f t="shared" ref="Y127:Y146" si="52">ABS(X127-W127)</f>
         <v>23.2849</v>
       </c>
       <c r="Z127" s="76" t="e">
@@ -14679,7 +14600,7 @@
       <c r="L151" s="3"/>
       <c r="M151" s="72">
         <f>AVERAGE(N3:N146)</f>
-        <v>44.718671679291944</v>
+        <v>43.794862155538205</v>
       </c>
       <c r="N151" s="6">
         <f>MIN(N3:N146)</f>
@@ -14687,7 +14608,7 @@
       </c>
       <c r="O151" s="7">
         <f>MAX(N3:N146)</f>
-        <v>167.48333333060145</v>
+        <v>58.716666667023674</v>
       </c>
       <c r="P151" s="5"/>
       <c r="T151" s="57"/>
@@ -14796,7 +14717,7 @@
       <c r="L154" s="3"/>
       <c r="M154" s="72">
         <f>AVERAGE(N3:P146)</f>
-        <v>44.007511737022853</v>
+        <v>43.142253521112664</v>
       </c>
       <c r="N154" s="6">
         <f>MIN(N3:O146)</f>
@@ -14804,7 +14725,7 @@
       </c>
       <c r="O154" s="7">
         <f>MAX(N3:O146)</f>
-        <v>167.48333333060145</v>
+        <v>58.716666667023674</v>
       </c>
       <c r="P154" s="5"/>
       <c r="T154" s="57"/>
@@ -15029,28 +14950,28 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="U1:V1 U2 U3:V1048576">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1 V3:V1048576">
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A147:P147 A3:R146">
-    <cfRule type="expression" dxfId="19" priority="34">
+    <cfRule type="expression" dxfId="7" priority="34">
       <formula>$P3&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="35">
+    <cfRule type="expression" dxfId="6" priority="35">
       <formula>$O3&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q147:R147">
-    <cfRule type="expression" dxfId="17" priority="76">
+    <cfRule type="expression" dxfId="5" priority="76">
       <formula>$P147&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="77">
+    <cfRule type="expression" dxfId="4" priority="77">
       <formula>$O166&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17864,17 +17785,17 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="N2 M2:M1048576">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:N65 B3:N26 B27:L28 N27:N28 B46:L62 N46:N62 M27:M62">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>$M3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:L45 N29:N45">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M29="Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
tickets created where needed
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-10.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-10.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13860" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13860"/>
   </bookViews>
   <sheets>
     <sheet name="Train Runs" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="432">
   <si>
     <t>Train ID</t>
   </si>
@@ -1305,9 +1305,6 @@
   </si>
   <si>
     <t>Poor GPS signal caused navigation issues as train approached DUS</t>
-  </si>
-  <si>
-    <t>Ticket Needed</t>
   </si>
   <si>
     <t>Premature downgrade, DUS Signal 20S</t>
@@ -1842,56 +1839,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -2253,8 +2201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK163"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A137" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R132" sqref="R132"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I146" sqref="I146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2654,10 +2602,10 @@
         <v>0.1</v>
       </c>
       <c r="Q5" s="62" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="R5" s="62" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="T5" s="75"/>
       <c r="U5" s="75"/>
@@ -2722,7 +2670,7 @@
       <c r="P6" s="13"/>
       <c r="Q6" s="62"/>
       <c r="R6" s="62" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="T6" s="75" t="str">
         <f t="shared" ref="T6:T37" si="4">"https://search-rtdc-monitor-bjffxe2xuh6vdkpspy63sjmuny.us-east-1.es.amazonaws.com/_plugin/kibana/#/discover/Steve-Slow-Train-Analysis-(2080s-and-2083s)?_g=(refreshInterval:(display:Off,section:0,value:0),time:(from:'"&amp;TEXT(E6-1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600',mode:absolute,to:'"&amp;TEXT(I6+1/24/60,"yyyy-MM-DD hh:mm:ss")&amp;"-0600'))&amp;_a=(columns:!(Source,'Data.Head%20End%20Milepost',Data.Speed,'Data.Locomotive%20State','Data.Train%20ID','Data.Warning%2FEnforcement%20Type','Data.Target%20Start%20Milepost','Data.Target%20Description','Data.Target%20Speed',"&amp;"'Data.Enforcement%20Train%20Speed','Data.Enforcement%20Start%20Milepost','Data.Target%20Type','Data.Enforcement%20Direction%20of%20Travel','Message%20ID','Data.Body%20of%20Summary%20Text'),filters:!(),index:'emp_*',interval:auto,query:"&amp;"(query_string:(analyze_wildcard:!t,query:'Message%5C%20ID:(2083%20OR%202080%20OR%201041)%20AND%20%22rtdc.l.rtdc."&amp;B6&amp;"%22')),sort:!(Time,asc))"</f>
@@ -5661,10 +5609,10 @@
         <v>43</v>
       </c>
       <c r="Q41" s="62" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="R41" s="62" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="T41" s="75" t="str">
         <f t="shared" si="13"/>
@@ -7252,10 +7200,10 @@
         <v>42.033333320869133</v>
       </c>
       <c r="Q60" s="62" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="R60" s="62" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="T60" s="75" t="str">
         <f t="shared" si="13"/>
@@ -7505,10 +7453,10 @@
         <v>39.183333325199783</v>
       </c>
       <c r="Q63" s="62" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="R63" s="62" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="T63" s="75" t="str">
         <f t="shared" si="13"/>
@@ -8348,10 +8296,10 @@
         <v>32.133333332603797</v>
       </c>
       <c r="Q73" s="62" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="R73" s="62" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="T73" s="75" t="str">
         <f t="shared" si="23"/>
@@ -9527,10 +9475,10 @@
         <v>36.033333332743496</v>
       </c>
       <c r="Q87" s="62" t="s">
+        <v>418</v>
+      </c>
+      <c r="R87" s="62" t="s">
         <v>419</v>
-      </c>
-      <c r="R87" s="62" t="s">
-        <v>420</v>
       </c>
       <c r="T87" s="75" t="str">
         <f t="shared" si="23"/>
@@ -9950,10 +9898,10 @@
         <v>23</v>
       </c>
       <c r="Q92" s="62" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="R92" s="62" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="T92" s="75" t="str">
         <f t="shared" si="31"/>
@@ -13313,10 +13261,10 @@
         <v>45</v>
       </c>
       <c r="Q132" s="62" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="R132" s="62" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="T132" s="75" t="str">
         <f t="shared" si="47"/>
@@ -14492,7 +14440,7 @@
         <v>41</v>
       </c>
       <c r="Q146" s="62" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="R146" s="62" t="s">
         <v>416</v>
@@ -15014,28 +14962,28 @@
     <mergeCell ref="A1:P1"/>
   </mergeCells>
   <conditionalFormatting sqref="U1:V1 U2 U3:V1048576">
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V1 V3:V1048576">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A147:P147 A3:R146">
-    <cfRule type="expression" dxfId="14" priority="34">
+    <cfRule type="expression" dxfId="7" priority="34">
       <formula>$P3&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="35">
+    <cfRule type="expression" dxfId="6" priority="35">
       <formula>$O3&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q147:R147">
-    <cfRule type="expression" dxfId="12" priority="76">
+    <cfRule type="expression" dxfId="5" priority="76">
       <formula>$P147&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="77">
+    <cfRule type="expression" dxfId="4" priority="77">
       <formula>$O166&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15067,7 +15015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -15194,7 +15142,7 @@
         <v>117</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -15239,7 +15187,7 @@
         <v>117</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -15327,7 +15275,7 @@
         <v>118</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -15845,7 +15793,7 @@
         <v>117</v>
       </c>
       <c r="N18" s="21" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -15890,7 +15838,7 @@
         <v>117</v>
       </c>
       <c r="N19" s="21" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -15935,7 +15883,7 @@
         <v>118</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -15980,7 +15928,7 @@
         <v>117</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16025,7 +15973,7 @@
         <v>118</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16070,7 +16018,7 @@
         <v>117</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16115,7 +16063,7 @@
         <v>117</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16160,7 +16108,7 @@
         <v>117</v>
       </c>
       <c r="N25" s="21" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="26" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -17871,17 +17819,17 @@
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="N2 M2:M1048576">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:N65 B27:L28 N27:N28 B46:L62 N46:N62 M27:M62 B3:N26">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>$M3="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:L45 N29:N45">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M29="Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>